<commit_message>
Manual journal template update
</commit_message>
<xml_diff>
--- a/input_templates/manual_journals_template.xlsx
+++ b/input_templates/manual_journals_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Entity</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Transaction Date</t>
+  </si>
+  <si>
+    <t>Debit</t>
   </si>
   <si>
     <t>Credit</t>
@@ -434,12 +437,14 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>